<commit_message>
Se removio mostrar interés al llenar formulario
</commit_message>
<xml_diff>
--- a/readme/Creditos y amortizaciones.xlsx
+++ b/readme/Creditos y amortizaciones.xlsx
@@ -1,24 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\FIDEGARANTE\Cartera2020\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\laravel\finance\readme\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{328F922A-7080-4E61-835A-1FCE6CA9CBDF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57578135-0CF8-47DA-8EA5-AAC4D77ED039}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A434DEBB-ABBB-BE42-8740-2D78E85532EE}"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{A434DEBB-ABBB-BE42-8740-2D78E85532EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -197,9 +208,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -262,31 +273,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="8" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -606,8 +617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0BFF399-1842-F048-B903-81541A1EAE3E}">
   <dimension ref="A1:S69"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -802,7 +813,7 @@
       </c>
       <c r="G9" s="10">
         <f ca="1">TODAY()+4</f>
-        <v>44313</v>
+        <v>45036</v>
       </c>
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
@@ -1009,7 +1020,7 @@
       </c>
       <c r="B17" s="14">
         <f ca="1">G9</f>
-        <v>44313</v>
+        <v>45036</v>
       </c>
       <c r="C17" s="11"/>
       <c r="D17" s="16"/>
@@ -1049,11 +1060,11 @@
       </c>
       <c r="B18" s="14">
         <f ca="1">B17</f>
-        <v>44313</v>
+        <v>45036</v>
       </c>
       <c r="C18" s="14">
         <f ca="1">DATE(YEAR(B18),MONTH(B18)+1,DAY(B18))</f>
-        <v>44343</v>
+        <v>45066</v>
       </c>
       <c r="D18" s="16">
         <f ca="1">C18-B18</f>
@@ -1098,11 +1109,11 @@
       </c>
       <c r="B19" s="14">
         <f ca="1">C18</f>
-        <v>44343</v>
+        <v>45066</v>
       </c>
       <c r="C19" s="14">
         <f t="shared" ref="C19:C29" ca="1" si="0">DATE(YEAR(B19),MONTH(B19)+1,DAY(B19))</f>
-        <v>44374</v>
+        <v>45097</v>
       </c>
       <c r="D19" s="16">
         <f t="shared" ref="D19:D29" ca="1" si="1">C19-B19</f>
@@ -1144,11 +1155,11 @@
       </c>
       <c r="B20" s="14">
         <f t="shared" ref="B20:B29" ca="1" si="6">C19</f>
-        <v>44374</v>
+        <v>45097</v>
       </c>
       <c r="C20" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>44404</v>
+        <v>45127</v>
       </c>
       <c r="D20" s="16">
         <f t="shared" ca="1" si="1"/>
@@ -1190,11 +1201,11 @@
       </c>
       <c r="B21" s="14">
         <f t="shared" ca="1" si="6"/>
-        <v>44404</v>
+        <v>45127</v>
       </c>
       <c r="C21" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>44435</v>
+        <v>45158</v>
       </c>
       <c r="D21" s="16">
         <f t="shared" ca="1" si="1"/>
@@ -1236,11 +1247,11 @@
       </c>
       <c r="B22" s="14">
         <f t="shared" ca="1" si="6"/>
-        <v>44435</v>
+        <v>45158</v>
       </c>
       <c r="C22" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>44466</v>
+        <v>45189</v>
       </c>
       <c r="D22" s="16">
         <f t="shared" ca="1" si="1"/>
@@ -1282,11 +1293,11 @@
       </c>
       <c r="B23" s="14">
         <f t="shared" ca="1" si="6"/>
-        <v>44466</v>
+        <v>45189</v>
       </c>
       <c r="C23" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>44496</v>
+        <v>45219</v>
       </c>
       <c r="D23" s="16">
         <f t="shared" ca="1" si="1"/>
@@ -1328,11 +1339,11 @@
       </c>
       <c r="B24" s="14">
         <f t="shared" ca="1" si="6"/>
-        <v>44496</v>
+        <v>45219</v>
       </c>
       <c r="C24" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>44527</v>
+        <v>45250</v>
       </c>
       <c r="D24" s="16">
         <f t="shared" ca="1" si="1"/>
@@ -1374,11 +1385,11 @@
       </c>
       <c r="B25" s="14">
         <f t="shared" ca="1" si="6"/>
-        <v>44527</v>
+        <v>45250</v>
       </c>
       <c r="C25" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>44557</v>
+        <v>45280</v>
       </c>
       <c r="D25" s="16">
         <f t="shared" ca="1" si="1"/>
@@ -1420,11 +1431,11 @@
       </c>
       <c r="B26" s="14">
         <f t="shared" ca="1" si="6"/>
-        <v>44557</v>
+        <v>45280</v>
       </c>
       <c r="C26" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>44588</v>
+        <v>45311</v>
       </c>
       <c r="D26" s="16">
         <f t="shared" ca="1" si="1"/>
@@ -1466,11 +1477,11 @@
       </c>
       <c r="B27" s="14">
         <f t="shared" ca="1" si="6"/>
-        <v>44588</v>
+        <v>45311</v>
       </c>
       <c r="C27" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>44619</v>
+        <v>45342</v>
       </c>
       <c r="D27" s="16">
         <f t="shared" ca="1" si="1"/>
@@ -1512,38 +1523,38 @@
       </c>
       <c r="B28" s="14">
         <f t="shared" ca="1" si="6"/>
-        <v>44619</v>
+        <v>45342</v>
       </c>
       <c r="C28" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>44647</v>
+        <v>45371</v>
       </c>
       <c r="D28" s="16">
         <f t="shared" ca="1" si="1"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E28" s="16"/>
       <c r="F28" s="16">
         <f t="shared" ca="1" si="7"/>
-        <v>4454.7716567302386</v>
+        <v>4457.7099695078632</v>
       </c>
       <c r="G28" s="16"/>
       <c r="H28" s="16">
         <f t="shared" ca="1" si="2"/>
-        <v>4360.1666761435945</v>
+        <v>4357.2283633659699</v>
       </c>
       <c r="I28" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>82.272757773489104</v>
+        <v>85.211070551113707</v>
       </c>
       <c r="J28" s="16"/>
       <c r="K28" s="16">
         <f t="shared" ca="1" si="4"/>
-        <v>13.163641243758256</v>
+        <v>13.633771288178194</v>
       </c>
       <c r="L28" s="16">
         <f t="shared" ca="1" si="5"/>
-        <v>4455.6030751608423</v>
+        <v>4456.0732052052617</v>
       </c>
       <c r="M28" s="16"/>
       <c r="N28" s="16"/>
@@ -1558,11 +1569,11 @@
       </c>
       <c r="B29" s="14">
         <f t="shared" ca="1" si="6"/>
-        <v>44647</v>
+        <v>45371</v>
       </c>
       <c r="C29" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>44678</v>
+        <v>45402</v>
       </c>
       <c r="D29" s="16">
         <f t="shared" ca="1" si="1"/>
@@ -1571,25 +1582,25 @@
       <c r="E29" s="16"/>
       <c r="F29" s="16">
         <f t="shared" ca="1" si="7"/>
-        <v>58.364863266033353</v>
+        <v>61.333538609027528</v>
       </c>
       <c r="G29" s="16"/>
       <c r="H29" s="16">
         <f t="shared" ca="1" si="2"/>
-        <v>4396.4067934642053</v>
+        <v>4396.3764308988357</v>
       </c>
       <c r="I29" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>46.032640452879129</v>
+        <v>46.063003018247919</v>
       </c>
       <c r="J29" s="16"/>
       <c r="K29" s="16">
         <f t="shared" ca="1" si="4"/>
-        <v>7.365222472460661</v>
+        <v>7.3700804829196676</v>
       </c>
       <c r="L29" s="16">
         <f t="shared" ca="1" si="5"/>
-        <v>4449.804656389545</v>
+        <v>4449.8095144000035</v>
       </c>
       <c r="M29" s="16"/>
       <c r="N29" s="16"/>
@@ -1635,7 +1646,7 @@
       </c>
       <c r="G31" s="6">
         <f ca="1">TODAY()+4</f>
-        <v>44313</v>
+        <v>45036</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
@@ -1731,7 +1742,7 @@
       </c>
       <c r="B39" s="1">
         <f ca="1">G31</f>
-        <v>44313</v>
+        <v>45036</v>
       </c>
       <c r="D39" s="3"/>
       <c r="E39" s="3">
@@ -1769,11 +1780,11 @@
       </c>
       <c r="B40" s="1">
         <f ca="1">B39</f>
-        <v>44313</v>
+        <v>45036</v>
       </c>
       <c r="C40" s="1">
         <f ca="1">DATE(YEAR(B40),MONTH(B40)+1,DAY(B40))</f>
-        <v>44343</v>
+        <v>45066</v>
       </c>
       <c r="D40" s="3">
         <f ca="1">C40-B40</f>
@@ -1814,11 +1825,11 @@
       </c>
       <c r="B41" s="1">
         <f ca="1">C40</f>
-        <v>44343</v>
+        <v>45066</v>
       </c>
       <c r="C41" s="1">
         <f t="shared" ref="C41:C51" ca="1" si="8">DATE(YEAR(B41),MONTH(B41)+1,DAY(B41))</f>
-        <v>44374</v>
+        <v>45097</v>
       </c>
       <c r="D41" s="3">
         <f t="shared" ref="D41:D51" ca="1" si="9">C41-B41</f>
@@ -1859,11 +1870,11 @@
       </c>
       <c r="B42" s="1">
         <f t="shared" ref="B42:B51" ca="1" si="13">C41</f>
-        <v>44374</v>
+        <v>45097</v>
       </c>
       <c r="C42" s="1">
         <f t="shared" ca="1" si="8"/>
-        <v>44404</v>
+        <v>45127</v>
       </c>
       <c r="D42" s="3">
         <f t="shared" ca="1" si="9"/>
@@ -1904,11 +1915,11 @@
       </c>
       <c r="B43" s="1">
         <f t="shared" ca="1" si="13"/>
-        <v>44404</v>
+        <v>45127</v>
       </c>
       <c r="C43" s="1">
         <f t="shared" ca="1" si="8"/>
-        <v>44435</v>
+        <v>45158</v>
       </c>
       <c r="D43" s="3">
         <f t="shared" ca="1" si="9"/>
@@ -1949,11 +1960,11 @@
       </c>
       <c r="B44" s="1">
         <f t="shared" ca="1" si="13"/>
-        <v>44435</v>
+        <v>45158</v>
       </c>
       <c r="C44" s="1">
         <f t="shared" ca="1" si="8"/>
-        <v>44466</v>
+        <v>45189</v>
       </c>
       <c r="D44" s="3">
         <f t="shared" ca="1" si="9"/>
@@ -1994,11 +2005,11 @@
       </c>
       <c r="B45" s="1">
         <f t="shared" ca="1" si="13"/>
-        <v>44466</v>
+        <v>45189</v>
       </c>
       <c r="C45" s="1">
         <f t="shared" ca="1" si="8"/>
-        <v>44496</v>
+        <v>45219</v>
       </c>
       <c r="D45" s="3">
         <f t="shared" ca="1" si="9"/>
@@ -2039,11 +2050,11 @@
       </c>
       <c r="B46" s="1">
         <f t="shared" ca="1" si="13"/>
-        <v>44496</v>
+        <v>45219</v>
       </c>
       <c r="C46" s="1">
         <f t="shared" ca="1" si="8"/>
-        <v>44527</v>
+        <v>45250</v>
       </c>
       <c r="D46" s="3">
         <f t="shared" ca="1" si="9"/>
@@ -2084,11 +2095,11 @@
       </c>
       <c r="B47" s="1">
         <f t="shared" ca="1" si="13"/>
-        <v>44527</v>
+        <v>45250</v>
       </c>
       <c r="C47" s="1">
         <f t="shared" ca="1" si="8"/>
-        <v>44557</v>
+        <v>45280</v>
       </c>
       <c r="D47" s="3">
         <f t="shared" ca="1" si="9"/>
@@ -2129,11 +2140,11 @@
       </c>
       <c r="B48" s="1">
         <f t="shared" ca="1" si="13"/>
-        <v>44557</v>
+        <v>45280</v>
       </c>
       <c r="C48" s="1">
         <f t="shared" ca="1" si="8"/>
-        <v>44588</v>
+        <v>45311</v>
       </c>
       <c r="D48" s="3">
         <f t="shared" ca="1" si="9"/>
@@ -2174,11 +2185,11 @@
       </c>
       <c r="B49" s="1">
         <f t="shared" ca="1" si="13"/>
-        <v>44588</v>
+        <v>45311</v>
       </c>
       <c r="C49" s="1">
         <f t="shared" ca="1" si="8"/>
-        <v>44619</v>
+        <v>45342</v>
       </c>
       <c r="D49" s="3">
         <f t="shared" ca="1" si="9"/>
@@ -2219,15 +2230,15 @@
       </c>
       <c r="B50" s="1">
         <f t="shared" ca="1" si="13"/>
-        <v>44619</v>
+        <v>45342</v>
       </c>
       <c r="C50" s="1">
         <f t="shared" ca="1" si="8"/>
-        <v>44647</v>
+        <v>45371</v>
       </c>
       <c r="D50" s="3">
         <f t="shared" ca="1" si="9"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E50" s="3"/>
       <c r="F50" s="3">
@@ -2241,16 +2252,16 @@
       </c>
       <c r="I50" s="3">
         <f t="shared" ca="1" si="10"/>
-        <v>77.7777777777778</v>
+        <v>80.555555555555571</v>
       </c>
       <c r="J50" s="3"/>
       <c r="K50" s="3">
         <f t="shared" ca="1" si="11"/>
-        <v>12.444444444444448</v>
+        <v>12.888888888888891</v>
       </c>
       <c r="L50" s="3">
         <f t="shared" ca="1" si="12"/>
-        <v>4256.8888888888887</v>
+        <v>4260.1111111111113</v>
       </c>
       <c r="M50" s="3"/>
       <c r="N50" s="3"/>
@@ -2264,11 +2275,11 @@
       </c>
       <c r="B51" s="1">
         <f t="shared" ca="1" si="13"/>
-        <v>44647</v>
+        <v>45371</v>
       </c>
       <c r="C51" s="1">
         <f t="shared" ca="1" si="8"/>
-        <v>44678</v>
+        <v>45402</v>
       </c>
       <c r="D51" s="3">
         <f t="shared" ca="1" si="9"/>
@@ -2313,7 +2324,7 @@
       </c>
       <c r="I52" s="4">
         <f ca="1">SUM(I39:I51)</f>
-        <v>3302.7777777777787</v>
+        <v>3305.5555555555566</v>
       </c>
       <c r="J52" s="4">
         <f>SUM(J39:J51)</f>
@@ -2321,11 +2332,11 @@
       </c>
       <c r="K52" s="4">
         <f ca="1">SUM(K39:K51)</f>
-        <v>608.44444444444457</v>
+        <v>608.88888888888903</v>
       </c>
       <c r="L52" s="4">
         <f ca="1">SUM(L40:L51)</f>
-        <v>53831.222222222226</v>
+        <v>53834.444444444445</v>
       </c>
     </row>
     <row r="54" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -2349,7 +2360,7 @@
       </c>
       <c r="G54" s="6">
         <f ca="1">TODAY()+4</f>
-        <v>44313</v>
+        <v>45036</v>
       </c>
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.25">
@@ -2439,7 +2450,7 @@
       </c>
       <c r="B62" s="1">
         <f ca="1">G54</f>
-        <v>44313</v>
+        <v>45036</v>
       </c>
       <c r="D62" s="3"/>
       <c r="E62" s="3">
@@ -2477,11 +2488,11 @@
       </c>
       <c r="B63" s="1">
         <f ca="1">B62</f>
-        <v>44313</v>
+        <v>45036</v>
       </c>
       <c r="C63" s="1">
         <f ca="1">DATE(YEAR(B63),MONTH(B63)+1,DAY(B63))</f>
-        <v>44343</v>
+        <v>45066</v>
       </c>
       <c r="D63" s="3">
         <f ca="1">C63-B63</f>
@@ -2521,11 +2532,11 @@
       </c>
       <c r="B64" s="1">
         <f ca="1">C63</f>
-        <v>44343</v>
+        <v>45066</v>
       </c>
       <c r="C64" s="1">
         <f ca="1">DATE(YEAR(B64),MONTH(B64)+1,DAY(B64))</f>
-        <v>44374</v>
+        <v>45097</v>
       </c>
       <c r="D64" s="3">
         <f ca="1">C64-B64</f>
@@ -2566,11 +2577,11 @@
       </c>
       <c r="B65" s="1">
         <f ca="1">C64</f>
-        <v>44374</v>
+        <v>45097</v>
       </c>
       <c r="C65" s="1">
         <f ca="1">DATE(YEAR(B65),MONTH(B65)+1,DAY(B65))</f>
-        <v>44404</v>
+        <v>45127</v>
       </c>
       <c r="D65" s="3">
         <f ca="1">C65-B65</f>

</xml_diff>

<commit_message>
Calcuo de créditos y amotización estable
</commit_message>
<xml_diff>
--- a/readme/Creditos y amortizaciones.xlsx
+++ b/readme/Creditos y amortizaciones.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\laravel\finance\readme\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57578135-0CF8-47DA-8EA5-AAC4D77ED039}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBE1D988-F1D5-4311-AAB8-9174879A6219}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{A434DEBB-ABBB-BE42-8740-2D78E85532EE}"/>
   </bookViews>
@@ -212,7 +212,7 @@
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -229,6 +229,14 @@
     </font>
     <font>
       <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -269,7 +277,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -300,6 +308,7 @@
     <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -617,8 +626,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0BFF399-1842-F048-B903-81541A1EAE3E}">
   <dimension ref="A1:S69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="K65" sqref="K65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -768,10 +777,6 @@
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
       <c r="H6" s="8"/>
-      <c r="I6" s="9">
-        <f>PMT(C13/12,C12,-C11,0,0)</f>
-        <v>4442.439433917084</v>
-      </c>
       <c r="J6" s="8"/>
       <c r="K6" s="8"/>
       <c r="L6" s="8"/>
@@ -813,7 +818,7 @@
       </c>
       <c r="G9" s="10">
         <f ca="1">TODAY()+4</f>
-        <v>45036</v>
+        <v>45037</v>
       </c>
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
@@ -897,7 +902,7 @@
       <c r="C13" s="12">
         <v>0.12</v>
       </c>
-      <c r="D13" s="11"/>
+      <c r="D13" s="20"/>
       <c r="E13" s="11"/>
       <c r="F13" s="11"/>
       <c r="G13" s="11"/>
@@ -916,7 +921,10 @@
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="11"/>
       <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
+      <c r="C14" s="9">
+        <f>PMT(C13/12,C12,-C11,0,0)</f>
+        <v>4442.439433917084</v>
+      </c>
       <c r="D14" s="11"/>
       <c r="E14" s="11"/>
       <c r="F14" s="11"/>
@@ -1020,7 +1028,7 @@
       </c>
       <c r="B17" s="14">
         <f ca="1">G9</f>
-        <v>45036</v>
+        <v>45037</v>
       </c>
       <c r="C17" s="11"/>
       <c r="D17" s="16"/>
@@ -1060,11 +1068,11 @@
       </c>
       <c r="B18" s="14">
         <f ca="1">B17</f>
-        <v>45036</v>
+        <v>45037</v>
       </c>
       <c r="C18" s="14">
         <f ca="1">DATE(YEAR(B18),MONTH(B18)+1,DAY(B18))</f>
-        <v>45066</v>
+        <v>45067</v>
       </c>
       <c r="D18" s="16">
         <f ca="1">C18-B18</f>
@@ -1090,7 +1098,7 @@
         <v>80.000000000000014</v>
       </c>
       <c r="L18" s="16">
-        <f ca="1">I$6+K18</f>
+        <f ca="1">C$14+K18</f>
         <v>4522.439433917084</v>
       </c>
       <c r="M18" s="18"/>
@@ -1109,11 +1117,11 @@
       </c>
       <c r="B19" s="14">
         <f ca="1">C18</f>
-        <v>45066</v>
+        <v>45067</v>
       </c>
       <c r="C19" s="14">
         <f t="shared" ref="C19:C29" ca="1" si="0">DATE(YEAR(B19),MONTH(B19)+1,DAY(B19))</f>
-        <v>45097</v>
+        <v>45098</v>
       </c>
       <c r="D19" s="16">
         <f t="shared" ref="D19:D29" ca="1" si="1">C19-B19</f>
@@ -1126,20 +1134,20 @@
       </c>
       <c r="G19" s="16"/>
       <c r="H19" s="16">
-        <f t="shared" ref="H19:H29" ca="1" si="2">I$6-I19</f>
+        <f ca="1">C$14-I19</f>
         <v>3966.5067672504174</v>
       </c>
       <c r="I19" s="16">
-        <f t="shared" ref="I19:I29" ca="1" si="3">F18*C$13/360*D19</f>
+        <f t="shared" ref="I19:I29" ca="1" si="2">F18*C$13/360*D19</f>
         <v>475.93266666666665</v>
       </c>
       <c r="J19" s="16"/>
       <c r="K19" s="16">
-        <f t="shared" ref="K19:K29" ca="1" si="4">(I19+J19+G19)*0.16</f>
+        <f t="shared" ref="K19:K29" ca="1" si="3">(I19+J19+G19)*0.16</f>
         <v>76.149226666666664</v>
       </c>
       <c r="L19" s="16">
-        <f t="shared" ref="L19:L29" ca="1" si="5">I$6+K19</f>
+        <f ca="1">C$14+K19</f>
         <v>4518.5886605837504</v>
       </c>
       <c r="M19" s="16"/>
@@ -1154,12 +1162,12 @@
         <v>3</v>
       </c>
       <c r="B20" s="14">
-        <f t="shared" ref="B20:B29" ca="1" si="6">C19</f>
-        <v>45097</v>
+        <f t="shared" ref="B20:B29" ca="1" si="4">C19</f>
+        <v>45098</v>
       </c>
       <c r="C20" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>45127</v>
+        <v>45128</v>
       </c>
       <c r="D20" s="16">
         <f t="shared" ca="1" si="1"/>
@@ -1167,25 +1175,25 @@
       </c>
       <c r="E20" s="16"/>
       <c r="F20" s="16">
-        <f t="shared" ref="F20:F29" ca="1" si="7">F19-H20</f>
+        <f ca="1">F19-H20</f>
         <v>38069.968731159999</v>
       </c>
       <c r="G20" s="16"/>
       <c r="H20" s="16">
+        <f ca="1">C$14-I20</f>
+        <v>4021.524501589588</v>
+      </c>
+      <c r="I20" s="16">
         <f t="shared" ca="1" si="2"/>
-        <v>4021.524501589588</v>
-      </c>
-      <c r="I20" s="16">
-        <f t="shared" ca="1" si="3"/>
         <v>420.91493232749582</v>
       </c>
       <c r="J20" s="16"/>
       <c r="K20" s="16">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="3"/>
         <v>67.346389172399327</v>
       </c>
       <c r="L20" s="16">
-        <f t="shared" ca="1" si="5"/>
+        <f ca="1">C$14+K20</f>
         <v>4509.7858230894835</v>
       </c>
       <c r="M20" s="16"/>
@@ -1200,12 +1208,12 @@
         <v>4</v>
       </c>
       <c r="B21" s="14">
-        <f t="shared" ca="1" si="6"/>
-        <v>45127</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>45128</v>
       </c>
       <c r="C21" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>45158</v>
+        <v>45159</v>
       </c>
       <c r="D21" s="16">
         <f t="shared" ca="1" si="1"/>
@@ -1213,25 +1221,25 @@
       </c>
       <c r="E21" s="16"/>
       <c r="F21" s="16">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ref="F20:F29" ca="1" si="5">F20-H21</f>
         <v>34020.918974131571</v>
       </c>
       <c r="G21" s="16"/>
       <c r="H21" s="16">
+        <f ca="1">C$14-I21</f>
+        <v>4049.0497570284306</v>
+      </c>
+      <c r="I21" s="16">
         <f t="shared" ca="1" si="2"/>
-        <v>4049.0497570284306</v>
-      </c>
-      <c r="I21" s="16">
-        <f t="shared" ca="1" si="3"/>
         <v>393.3896768886533</v>
       </c>
       <c r="J21" s="16"/>
       <c r="K21" s="16">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="3"/>
         <v>62.942348302184527</v>
       </c>
       <c r="L21" s="16">
-        <f t="shared" ca="1" si="5"/>
+        <f ca="1">C$14+K21</f>
         <v>4505.3817822192686</v>
       </c>
       <c r="M21" s="16"/>
@@ -1246,12 +1254,12 @@
         <v>5</v>
       </c>
       <c r="B22" s="14">
-        <f t="shared" ca="1" si="6"/>
-        <v>45158</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>45159</v>
       </c>
       <c r="C22" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>45189</v>
+        <v>45190</v>
       </c>
       <c r="D22" s="16">
         <f t="shared" ca="1" si="1"/>
@@ -1259,25 +1267,25 @@
       </c>
       <c r="E22" s="16"/>
       <c r="F22" s="16">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="5"/>
         <v>29930.029036280514</v>
       </c>
       <c r="G22" s="16"/>
       <c r="H22" s="16">
+        <f ca="1">C$14-I22</f>
+        <v>4090.8899378510578</v>
+      </c>
+      <c r="I22" s="16">
         <f t="shared" ca="1" si="2"/>
-        <v>4090.8899378510578</v>
-      </c>
-      <c r="I22" s="16">
-        <f t="shared" ca="1" si="3"/>
         <v>351.54949606602622</v>
       </c>
       <c r="J22" s="16"/>
       <c r="K22" s="16">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="3"/>
         <v>56.247919370564198</v>
       </c>
       <c r="L22" s="16">
-        <f t="shared" ca="1" si="5"/>
+        <f ca="1">C$14+K22</f>
         <v>4498.687353287648</v>
       </c>
       <c r="M22" s="16"/>
@@ -1292,12 +1300,12 @@
         <v>6</v>
       </c>
       <c r="B23" s="14">
-        <f t="shared" ca="1" si="6"/>
-        <v>45189</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>45190</v>
       </c>
       <c r="C23" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>45219</v>
+        <v>45220</v>
       </c>
       <c r="D23" s="16">
         <f t="shared" ca="1" si="1"/>
@@ -1305,25 +1313,25 @@
       </c>
       <c r="E23" s="16"/>
       <c r="F23" s="16">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="5"/>
         <v>25786.889892726234</v>
       </c>
       <c r="G23" s="16"/>
       <c r="H23" s="16">
+        <f ca="1">C$14-I23</f>
+        <v>4143.1391435542791</v>
+      </c>
+      <c r="I23" s="16">
         <f t="shared" ca="1" si="2"/>
-        <v>4143.1391435542791</v>
-      </c>
-      <c r="I23" s="16">
-        <f t="shared" ca="1" si="3"/>
         <v>299.30029036280513</v>
       </c>
       <c r="J23" s="16"/>
       <c r="K23" s="16">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="3"/>
         <v>47.888046458048819</v>
       </c>
       <c r="L23" s="16">
-        <f t="shared" ca="1" si="5"/>
+        <f ca="1">C$14+K23</f>
         <v>4490.3274803751328</v>
       </c>
       <c r="M23" s="16"/>
@@ -1338,12 +1346,12 @@
         <v>7</v>
       </c>
       <c r="B24" s="14">
-        <f t="shared" ca="1" si="6"/>
-        <v>45219</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>45220</v>
       </c>
       <c r="C24" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>45250</v>
+        <v>45251</v>
       </c>
       <c r="D24" s="16">
         <f t="shared" ca="1" si="1"/>
@@ -1351,25 +1359,25 @@
       </c>
       <c r="E24" s="16"/>
       <c r="F24" s="16">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="5"/>
         <v>21610.914987700657</v>
       </c>
       <c r="G24" s="16"/>
       <c r="H24" s="16">
+        <f ca="1">C$14-I24</f>
+        <v>4175.9749050255796</v>
+      </c>
+      <c r="I24" s="16">
         <f t="shared" ca="1" si="2"/>
-        <v>4175.9749050255796</v>
-      </c>
-      <c r="I24" s="16">
-        <f t="shared" ca="1" si="3"/>
         <v>266.46452889150441</v>
       </c>
       <c r="J24" s="16"/>
       <c r="K24" s="16">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="3"/>
         <v>42.634324622640705</v>
       </c>
       <c r="L24" s="16">
-        <f t="shared" ca="1" si="5"/>
+        <f ca="1">C$14+K24</f>
         <v>4485.0737585397246</v>
       </c>
       <c r="M24" s="16"/>
@@ -1384,12 +1392,12 @@
         <v>8</v>
       </c>
       <c r="B25" s="14">
-        <f t="shared" ca="1" si="6"/>
-        <v>45250</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>45251</v>
       </c>
       <c r="C25" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>45280</v>
+        <v>45281</v>
       </c>
       <c r="D25" s="16">
         <f t="shared" ca="1" si="1"/>
@@ -1397,25 +1405,25 @@
       </c>
       <c r="E25" s="16"/>
       <c r="F25" s="16">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="5"/>
         <v>17384.584703660577</v>
       </c>
       <c r="G25" s="16"/>
       <c r="H25" s="16">
+        <f ca="1">C$14-I25</f>
+        <v>4226.3302840400775</v>
+      </c>
+      <c r="I25" s="16">
         <f t="shared" ca="1" si="2"/>
-        <v>4226.3302840400775</v>
-      </c>
-      <c r="I25" s="16">
-        <f t="shared" ca="1" si="3"/>
         <v>216.10914987700656</v>
       </c>
       <c r="J25" s="16"/>
       <c r="K25" s="16">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="3"/>
         <v>34.577463980321049</v>
       </c>
       <c r="L25" s="16">
-        <f t="shared" ca="1" si="5"/>
+        <f ca="1">C$14+K25</f>
         <v>4477.0168978974052</v>
       </c>
       <c r="M25" s="16"/>
@@ -1430,12 +1438,12 @@
         <v>9</v>
       </c>
       <c r="B26" s="14">
-        <f t="shared" ca="1" si="6"/>
-        <v>45280</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>45281</v>
       </c>
       <c r="C26" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>45311</v>
+        <v>45312</v>
       </c>
       <c r="D26" s="16">
         <f t="shared" ca="1" si="1"/>
@@ -1443,25 +1451,25 @@
       </c>
       <c r="E26" s="16"/>
       <c r="F26" s="16">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="5"/>
         <v>13121.785978347987</v>
       </c>
       <c r="G26" s="16"/>
       <c r="H26" s="16">
+        <f ca="1">C$14-I26</f>
+        <v>4262.7987253125912</v>
+      </c>
+      <c r="I26" s="16">
         <f t="shared" ca="1" si="2"/>
-        <v>4262.7987253125912</v>
-      </c>
-      <c r="I26" s="16">
-        <f t="shared" ca="1" si="3"/>
         <v>179.64070860449263</v>
       </c>
       <c r="J26" s="16"/>
       <c r="K26" s="16">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="3"/>
         <v>28.742513376718822</v>
       </c>
       <c r="L26" s="16">
-        <f t="shared" ca="1" si="5"/>
+        <f ca="1">C$14+K26</f>
         <v>4471.1819472938032</v>
       </c>
       <c r="M26" s="16"/>
@@ -1476,12 +1484,12 @@
         <v>10</v>
       </c>
       <c r="B27" s="14">
-        <f t="shared" ca="1" si="6"/>
-        <v>45311</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>45312</v>
       </c>
       <c r="C27" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>45342</v>
+        <v>45343</v>
       </c>
       <c r="D27" s="16">
         <f t="shared" ca="1" si="1"/>
@@ -1489,25 +1497,25 @@
       </c>
       <c r="E27" s="16"/>
       <c r="F27" s="16">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="5"/>
         <v>8814.9383328738331</v>
       </c>
       <c r="G27" s="16"/>
       <c r="H27" s="16">
+        <f ca="1">C$14-I27</f>
+        <v>4306.8476454741549</v>
+      </c>
+      <c r="I27" s="16">
         <f t="shared" ca="1" si="2"/>
-        <v>4306.8476454741549</v>
-      </c>
-      <c r="I27" s="16">
-        <f t="shared" ca="1" si="3"/>
         <v>135.59178844292921</v>
       </c>
       <c r="J27" s="16"/>
       <c r="K27" s="16">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="3"/>
         <v>21.694686150868673</v>
       </c>
       <c r="L27" s="16">
-        <f t="shared" ca="1" si="5"/>
+        <f ca="1">C$14+K27</f>
         <v>4464.1341200679526</v>
       </c>
       <c r="M27" s="16"/>
@@ -1522,12 +1530,12 @@
         <v>11</v>
       </c>
       <c r="B28" s="14">
-        <f t="shared" ca="1" si="6"/>
-        <v>45342</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>45343</v>
       </c>
       <c r="C28" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>45371</v>
+        <v>45372</v>
       </c>
       <c r="D28" s="16">
         <f t="shared" ca="1" si="1"/>
@@ -1535,25 +1543,25 @@
       </c>
       <c r="E28" s="16"/>
       <c r="F28" s="16">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="5"/>
         <v>4457.7099695078632</v>
       </c>
       <c r="G28" s="16"/>
       <c r="H28" s="16">
+        <f ca="1">C$14-I28</f>
+        <v>4357.2283633659699</v>
+      </c>
+      <c r="I28" s="16">
         <f t="shared" ca="1" si="2"/>
-        <v>4357.2283633659699</v>
-      </c>
-      <c r="I28" s="16">
-        <f t="shared" ca="1" si="3"/>
         <v>85.211070551113707</v>
       </c>
       <c r="J28" s="16"/>
       <c r="K28" s="16">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="3"/>
         <v>13.633771288178194</v>
       </c>
       <c r="L28" s="16">
-        <f t="shared" ca="1" si="5"/>
+        <f ca="1">C$14+K28</f>
         <v>4456.0732052052617</v>
       </c>
       <c r="M28" s="16"/>
@@ -1568,12 +1576,12 @@
         <v>12</v>
       </c>
       <c r="B29" s="14">
-        <f t="shared" ca="1" si="6"/>
-        <v>45371</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>45372</v>
       </c>
       <c r="C29" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>45402</v>
+        <v>45403</v>
       </c>
       <c r="D29" s="16">
         <f t="shared" ca="1" si="1"/>
@@ -1581,25 +1589,25 @@
       </c>
       <c r="E29" s="16"/>
       <c r="F29" s="16">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="5"/>
         <v>61.333538609027528</v>
       </c>
       <c r="G29" s="16"/>
       <c r="H29" s="16">
+        <f ca="1">C$14-I29</f>
+        <v>4396.3764308988357</v>
+      </c>
+      <c r="I29" s="16">
         <f t="shared" ca="1" si="2"/>
-        <v>4396.3764308988357</v>
-      </c>
-      <c r="I29" s="16">
-        <f t="shared" ca="1" si="3"/>
         <v>46.063003018247919</v>
       </c>
       <c r="J29" s="16"/>
       <c r="K29" s="16">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="3"/>
         <v>7.3700804829196676</v>
       </c>
       <c r="L29" s="16">
-        <f t="shared" ca="1" si="5"/>
+        <f ca="1">C$14+K29</f>
         <v>4449.8095144000035</v>
       </c>
       <c r="M29" s="16"/>
@@ -1646,7 +1654,7 @@
       </c>
       <c r="G31" s="6">
         <f ca="1">TODAY()+4</f>
-        <v>45036</v>
+        <v>45037</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
@@ -1742,7 +1750,7 @@
       </c>
       <c r="B39" s="1">
         <f ca="1">G31</f>
-        <v>45036</v>
+        <v>45037</v>
       </c>
       <c r="D39" s="3"/>
       <c r="E39" s="3">
@@ -1780,11 +1788,11 @@
       </c>
       <c r="B40" s="1">
         <f ca="1">B39</f>
-        <v>45036</v>
+        <v>45037</v>
       </c>
       <c r="C40" s="1">
         <f ca="1">DATE(YEAR(B40),MONTH(B40)+1,DAY(B40))</f>
-        <v>45066</v>
+        <v>45067</v>
       </c>
       <c r="D40" s="3">
         <f ca="1">C40-B40</f>
@@ -1825,14 +1833,14 @@
       </c>
       <c r="B41" s="1">
         <f ca="1">C40</f>
-        <v>45066</v>
+        <v>45067</v>
       </c>
       <c r="C41" s="1">
-        <f t="shared" ref="C41:C51" ca="1" si="8">DATE(YEAR(B41),MONTH(B41)+1,DAY(B41))</f>
-        <v>45097</v>
+        <f t="shared" ref="C41:C51" ca="1" si="6">DATE(YEAR(B41),MONTH(B41)+1,DAY(B41))</f>
+        <v>45098</v>
       </c>
       <c r="D41" s="3">
-        <f t="shared" ref="D41:D51" ca="1" si="9">C41-B41</f>
+        <f t="shared" ref="D41:D51" ca="1" si="7">C41-B41</f>
         <v>31</v>
       </c>
       <c r="E41" s="3"/>
@@ -1846,16 +1854,16 @@
         <v>4166.666666666667</v>
       </c>
       <c r="I41" s="3">
-        <f t="shared" ref="I41:I51" ca="1" si="10">F40*C$13/360*D41</f>
+        <f t="shared" ref="I41:I51" ca="1" si="8">F40*C$13/360*D41</f>
         <v>473.61111111111114</v>
       </c>
       <c r="J41" s="3"/>
       <c r="K41" s="3">
-        <f t="shared" ref="K41:K51" ca="1" si="11">(I41+J41+G41)*0.16</f>
+        <f t="shared" ref="K41:K51" ca="1" si="9">(I41+J41+G41)*0.16</f>
         <v>75.777777777777786</v>
       </c>
       <c r="L41" s="3">
-        <f t="shared" ref="L41:L51" ca="1" si="12">SUM(G41:K41)</f>
+        <f t="shared" ref="L41:L51" ca="1" si="10">SUM(G41:K41)</f>
         <v>4716.0555555555557</v>
       </c>
       <c r="M41" s="3"/>
@@ -1869,38 +1877,38 @@
         <v>3</v>
       </c>
       <c r="B42" s="1">
-        <f t="shared" ref="B42:B51" ca="1" si="13">C41</f>
-        <v>45097</v>
+        <f t="shared" ref="B42:B51" ca="1" si="11">C41</f>
+        <v>45098</v>
       </c>
       <c r="C42" s="1">
-        <f t="shared" ca="1" si="8"/>
-        <v>45127</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>45128</v>
       </c>
       <c r="D42" s="3">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="7"/>
         <v>30</v>
       </c>
       <c r="E42" s="3"/>
       <c r="F42" s="3">
-        <f t="shared" ref="F42:F51" si="14">F41-H42</f>
+        <f t="shared" ref="F42:F51" si="12">F41-H42</f>
         <v>37500.000000000007</v>
       </c>
       <c r="G42" s="3"/>
       <c r="H42" s="3">
-        <f t="shared" ref="H42:H51" si="15">H41</f>
+        <f t="shared" ref="H42:H51" si="13">H41</f>
         <v>4166.666666666667</v>
       </c>
       <c r="I42" s="3">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="8"/>
         <v>416.66666666666669</v>
       </c>
       <c r="J42" s="3"/>
       <c r="K42" s="3">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="9"/>
         <v>66.666666666666671</v>
       </c>
       <c r="L42" s="3">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="10"/>
         <v>4650.0000000000009</v>
       </c>
       <c r="M42" s="3"/>
@@ -1914,38 +1922,38 @@
         <v>4</v>
       </c>
       <c r="B43" s="1">
-        <f t="shared" ca="1" si="13"/>
-        <v>45127</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>45128</v>
       </c>
       <c r="C43" s="1">
-        <f t="shared" ca="1" si="8"/>
-        <v>45158</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>45159</v>
       </c>
       <c r="D43" s="3">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="7"/>
         <v>31</v>
       </c>
       <c r="E43" s="3"/>
       <c r="F43" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>33333.333333333343</v>
       </c>
       <c r="G43" s="3"/>
       <c r="H43" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>4166.666666666667</v>
       </c>
       <c r="I43" s="3">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="8"/>
         <v>387.50000000000006</v>
       </c>
       <c r="J43" s="3"/>
       <c r="K43" s="3">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="9"/>
         <v>62.000000000000007</v>
       </c>
       <c r="L43" s="3">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="10"/>
         <v>4616.166666666667</v>
       </c>
       <c r="M43" s="3"/>
@@ -1959,38 +1967,38 @@
         <v>5</v>
       </c>
       <c r="B44" s="1">
-        <f t="shared" ca="1" si="13"/>
-        <v>45158</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>45159</v>
       </c>
       <c r="C44" s="1">
-        <f t="shared" ca="1" si="8"/>
-        <v>45189</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>45190</v>
       </c>
       <c r="D44" s="3">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="7"/>
         <v>31</v>
       </c>
       <c r="E44" s="3"/>
       <c r="F44" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>29166.666666666675</v>
       </c>
       <c r="G44" s="3"/>
       <c r="H44" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>4166.666666666667</v>
       </c>
       <c r="I44" s="3">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="8"/>
         <v>344.44444444444457</v>
       </c>
       <c r="J44" s="3"/>
       <c r="K44" s="3">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="9"/>
         <v>55.111111111111136</v>
       </c>
       <c r="L44" s="3">
-        <f t="shared" ca="1" si="12"/>
+        <f ca="1">SUM(G44:K44)</f>
         <v>4566.2222222222226</v>
       </c>
       <c r="M44" s="3"/>
@@ -2004,38 +2012,38 @@
         <v>6</v>
       </c>
       <c r="B45" s="1">
-        <f t="shared" ca="1" si="13"/>
-        <v>45189</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>45190</v>
       </c>
       <c r="C45" s="1">
-        <f t="shared" ca="1" si="8"/>
-        <v>45219</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>45220</v>
       </c>
       <c r="D45" s="3">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="7"/>
         <v>30</v>
       </c>
       <c r="E45" s="3"/>
       <c r="F45" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>25000.000000000007</v>
       </c>
       <c r="G45" s="3"/>
       <c r="H45" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>4166.666666666667</v>
       </c>
       <c r="I45" s="3">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="8"/>
         <v>291.66666666666674</v>
       </c>
       <c r="J45" s="3"/>
       <c r="K45" s="3">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="9"/>
         <v>46.666666666666679</v>
       </c>
       <c r="L45" s="3">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="10"/>
         <v>4505.0000000000009</v>
       </c>
       <c r="M45" s="3"/>
@@ -2049,38 +2057,38 @@
         <v>7</v>
       </c>
       <c r="B46" s="1">
-        <f t="shared" ca="1" si="13"/>
-        <v>45219</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>45220</v>
       </c>
       <c r="C46" s="1">
-        <f t="shared" ca="1" si="8"/>
-        <v>45250</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>45251</v>
       </c>
       <c r="D46" s="3">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="7"/>
         <v>31</v>
       </c>
       <c r="E46" s="3"/>
       <c r="F46" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>20833.333333333339</v>
       </c>
       <c r="G46" s="3"/>
       <c r="H46" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>4166.666666666667</v>
       </c>
       <c r="I46" s="3">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="8"/>
         <v>258.33333333333343</v>
       </c>
       <c r="J46" s="3"/>
       <c r="K46" s="3">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="9"/>
         <v>41.33333333333335</v>
       </c>
       <c r="L46" s="3">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="10"/>
         <v>4466.333333333333</v>
       </c>
       <c r="M46" s="3"/>
@@ -2094,38 +2102,38 @@
         <v>8</v>
       </c>
       <c r="B47" s="1">
-        <f t="shared" ca="1" si="13"/>
-        <v>45250</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>45251</v>
       </c>
       <c r="C47" s="1">
-        <f t="shared" ca="1" si="8"/>
-        <v>45280</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>45281</v>
       </c>
       <c r="D47" s="3">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="7"/>
         <v>30</v>
       </c>
       <c r="E47" s="3"/>
       <c r="F47" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>16666.666666666672</v>
       </c>
       <c r="G47" s="3"/>
       <c r="H47" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>4166.666666666667</v>
       </c>
       <c r="I47" s="3">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="8"/>
         <v>208.33333333333337</v>
       </c>
       <c r="J47" s="3"/>
       <c r="K47" s="3">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="9"/>
         <v>33.333333333333343</v>
       </c>
       <c r="L47" s="3">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="10"/>
         <v>4408.333333333333</v>
       </c>
       <c r="M47" s="3"/>
@@ -2139,38 +2147,38 @@
         <v>9</v>
       </c>
       <c r="B48" s="1">
-        <f t="shared" ca="1" si="13"/>
-        <v>45280</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>45281</v>
       </c>
       <c r="C48" s="1">
-        <f t="shared" ca="1" si="8"/>
-        <v>45311</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>45312</v>
       </c>
       <c r="D48" s="3">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="7"/>
         <v>31</v>
       </c>
       <c r="E48" s="3"/>
       <c r="F48" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>12500.000000000004</v>
       </c>
       <c r="G48" s="3"/>
       <c r="H48" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>4166.666666666667</v>
       </c>
       <c r="I48" s="3">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="8"/>
         <v>172.22222222222229</v>
       </c>
       <c r="J48" s="3"/>
       <c r="K48" s="3">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="9"/>
         <v>27.555555555555568</v>
       </c>
       <c r="L48" s="3">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="10"/>
         <v>4366.4444444444453</v>
       </c>
       <c r="M48" s="3"/>
@@ -2184,38 +2192,38 @@
         <v>10</v>
       </c>
       <c r="B49" s="1">
-        <f t="shared" ca="1" si="13"/>
-        <v>45311</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>45312</v>
       </c>
       <c r="C49" s="1">
-        <f t="shared" ca="1" si="8"/>
-        <v>45342</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>45343</v>
       </c>
       <c r="D49" s="3">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="7"/>
         <v>31</v>
       </c>
       <c r="E49" s="3"/>
       <c r="F49" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>8333.3333333333358</v>
       </c>
       <c r="G49" s="3"/>
       <c r="H49" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>4166.666666666667</v>
       </c>
       <c r="I49" s="3">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="8"/>
         <v>129.16666666666671</v>
       </c>
       <c r="J49" s="3"/>
       <c r="K49" s="3">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="9"/>
         <v>20.666666666666675</v>
       </c>
       <c r="L49" s="3">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="10"/>
         <v>4316.5000000000009</v>
       </c>
       <c r="M49" s="3"/>
@@ -2229,38 +2237,38 @@
         <v>11</v>
       </c>
       <c r="B50" s="1">
-        <f t="shared" ca="1" si="13"/>
-        <v>45342</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>45343</v>
       </c>
       <c r="C50" s="1">
-        <f t="shared" ca="1" si="8"/>
-        <v>45371</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>45372</v>
       </c>
       <c r="D50" s="3">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="7"/>
         <v>29</v>
       </c>
       <c r="E50" s="3"/>
       <c r="F50" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>4166.6666666666688</v>
       </c>
       <c r="G50" s="3"/>
       <c r="H50" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>4166.666666666667</v>
       </c>
       <c r="I50" s="3">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="8"/>
         <v>80.555555555555571</v>
       </c>
       <c r="J50" s="3"/>
       <c r="K50" s="3">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="9"/>
         <v>12.888888888888891</v>
       </c>
       <c r="L50" s="3">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="10"/>
         <v>4260.1111111111113</v>
       </c>
       <c r="M50" s="3"/>
@@ -2274,38 +2282,38 @@
         <v>12</v>
       </c>
       <c r="B51" s="1">
-        <f t="shared" ca="1" si="13"/>
-        <v>45371</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>45372</v>
       </c>
       <c r="C51" s="1">
-        <f t="shared" ca="1" si="8"/>
-        <v>45402</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>45403</v>
       </c>
       <c r="D51" s="3">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="7"/>
         <v>31</v>
       </c>
       <c r="E51" s="3"/>
       <c r="F51" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="G51" s="3"/>
       <c r="H51" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>4166.666666666667</v>
       </c>
       <c r="I51" s="3">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="8"/>
         <v>43.055555555555571</v>
       </c>
       <c r="J51" s="3"/>
       <c r="K51" s="3">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="9"/>
         <v>6.8888888888888919</v>
       </c>
       <c r="L51" s="3">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="10"/>
         <v>4216.6111111111113</v>
       </c>
       <c r="M51" s="3"/>
@@ -2360,7 +2368,7 @@
       </c>
       <c r="G54" s="6">
         <f ca="1">TODAY()+4</f>
-        <v>45036</v>
+        <v>45037</v>
       </c>
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.25">
@@ -2450,7 +2458,7 @@
       </c>
       <c r="B62" s="1">
         <f ca="1">G54</f>
-        <v>45036</v>
+        <v>45037</v>
       </c>
       <c r="D62" s="3"/>
       <c r="E62" s="3">
@@ -2488,11 +2496,11 @@
       </c>
       <c r="B63" s="1">
         <f ca="1">B62</f>
-        <v>45036</v>
+        <v>45037</v>
       </c>
       <c r="C63" s="1">
         <f ca="1">DATE(YEAR(B63),MONTH(B63)+1,DAY(B63))</f>
-        <v>45066</v>
+        <v>45067</v>
       </c>
       <c r="D63" s="3">
         <f ca="1">C63-B63</f>
@@ -2532,11 +2540,11 @@
       </c>
       <c r="B64" s="1">
         <f ca="1">C63</f>
-        <v>45066</v>
+        <v>45067</v>
       </c>
       <c r="C64" s="1">
         <f ca="1">DATE(YEAR(B64),MONTH(B64)+1,DAY(B64))</f>
-        <v>45097</v>
+        <v>45098</v>
       </c>
       <c r="D64" s="3">
         <f ca="1">C64-B64</f>
@@ -2577,11 +2585,11 @@
       </c>
       <c r="B65" s="1">
         <f ca="1">C64</f>
-        <v>45097</v>
+        <v>45098</v>
       </c>
       <c r="C65" s="1">
         <f ca="1">DATE(YEAR(B65),MONTH(B65)+1,DAY(B65))</f>
-        <v>45127</v>
+        <v>45128</v>
       </c>
       <c r="D65" s="3">
         <f ca="1">C65-B65</f>
@@ -2653,5 +2661,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>